<commit_message>
Addition of prerequisites and limitations
</commit_message>
<xml_diff>
--- a/Documentation/PTP_Jean_Ramirez_Alejandor_Marin_26092023.xlsx
+++ b/Documentation/PTP_Jean_Ramirez_Alejandor_Marin_26092023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutomatizacionPrueba\Documents\Senasoft2023Grupo1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7095B252-851C-4AB5-B6B2-8944B45C29E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6CE750-6E8B-4FE5-9EA5-7999D4FAF1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scope" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,36 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Prerequisites</t>
+  </si>
+  <si>
+    <t>That the web page is working.
+That the manual tests have been successful.
+Intellij IDEA Community
+Gradle v6.8
+JDK v11
+Chrome
+Chromedriver
+Plugins:
+  Cucumber for Java
+  Gherkin
+Have internet</t>
+  </si>
+  <si>
+    <t>Limitations</t>
+  </si>
+  <si>
+    <t>We have 30mbps navigation.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,16 +66,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -56,12 +97,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,11 +431,66 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74755183-3FF7-445A-9C76-DE7DF0524AEF}">
+  <dimension ref="C2:C3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7B88FB-105A-4D83-ADA3-ECB983E6D61B}">
+  <dimension ref="C2:C3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4997E7-E7E9-4DDB-AF0E-D791DECFBEB6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -378,8 +498,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7B88FB-105A-4D83-ADA3-ECB983E6D61B}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBDF157-B67E-47D3-9BD0-13E1010331DB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -388,28 +508,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4997E7-E7E9-4DDB-AF0E-D791DECFBEB6}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBDF157-B67E-47D3-9BD0-13E1010331DB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add the scope and strategy
</commit_message>
<xml_diff>
--- a/Documentation/PTP_Jean_Ramirez_Alejandor_Marin_26092023.xlsx
+++ b/Documentation/PTP_Jean_Ramirez_Alejandor_Marin_26092023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutomatizacionPrueba\Documents\Senasoft2023Grupo1\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Autmotizacion_Prueba\Documents\Senasoft2023Grupo1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7095B252-851C-4AB5-B6B2-8944B45C29E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498F3A9E-56F0-478A-BF3E-344A921C1983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scope" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,173 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+  <si>
+    <t>Validate user registration module</t>
+  </si>
+  <si>
+    <t>Validate user login module</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Out of reach</t>
+  </si>
+  <si>
+    <t>Validate the following sections: booking &amp; trips, genius loyalty program, reward &amp; wallet.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: offers, trending destinations, explore Colombia, browse by property type, quick and easy trip planner, get inspiration for your next trip, saty at our top unique properties, home guests love, destinations we love, suscribe and footer.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: popular rental car companies, frequently asked questions, popular car rental destinations, suscribe and footer.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: nearby destinations, explore more destinations and footer.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: airport taxis for any kind of trip, learn more about our airport taxi service and footer.</t>
+  </si>
+  <si>
+    <t>Not all languages will be validated in this section, only the change from Spanish to English and Spanish to French will be performed.</t>
+  </si>
+  <si>
+    <t>Not all currencies in this section will be validated, only U.S. dollar(USD) and euro(EUR) will be selected.</t>
+  </si>
+  <si>
+    <t>Validate accommodation search module</t>
+  </si>
+  <si>
+    <t>Validate flight search module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate car rental module </t>
+  </si>
+  <si>
+    <t>Validate attractions module</t>
+  </si>
+  <si>
+    <t>Validate cab reservation module</t>
+  </si>
+  <si>
+    <t>Validate language selector</t>
+  </si>
+  <si>
+    <t>Validate currency selector</t>
+  </si>
+  <si>
+    <t>Validate account management dropdown</t>
+  </si>
+  <si>
+    <t>limpiar busqueda al refrescar la pagina</t>
+  </si>
+  <si>
+    <t>si cierro sesion y doy volver, el nombre se conserva en la pantalla de bienvenida</t>
+  </si>
+  <si>
+    <t>el "a tener en cuenta" no redirecciona hacia la seccion</t>
+  </si>
+  <si>
+    <t>hotel albura no cuenta con con link de redireccion "a tener en cuenta", a pesar de tener la seccion</t>
+  </si>
+  <si>
+    <t>selector de moneda presenta error en el area de gestion de cuenta</t>
+  </si>
+  <si>
+    <t>cuando se selecciona una moneda en "gestion de cuentas" al salir del area no conserva la selección</t>
+  </si>
+  <si>
+    <t>cuando se selecciona un destino, no se borra al refrescar la pagina, ni al cerrar sesion</t>
+  </si>
+  <si>
+    <t>simbolo de moneda en monedero permanece en simbolo euro</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the accommodation search page.</t>
+  </si>
+  <si>
+    <t>selector de moneda desaparece en modulo de vuelos</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: flight type selectors, popular flights near you, trending cities, fly worldwide with booking.com and footer</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the flight page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the entered email address is not already registered </t>
+  </si>
+  <si>
+    <t>Validate that if the password entered does not have uppercase, lowercase and minimum 10 characters, do not allow to create the account.</t>
+  </si>
+  <si>
+    <t>Validate not to allow to create a user if a mandatory field is blank</t>
+  </si>
+  <si>
+    <t>Validate that the user cannot log in if he/she does not have valid credentials</t>
+  </si>
+  <si>
+    <t>Validate that the user can enter information in the search bar according to the place he/she wishes to travel to</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the departure airport, destination airport and dates.</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the car rental page.</t>
+  </si>
+  <si>
+    <t>al ingresar al selector de idiomas se observa la bandera de colombia para español de mexico y español argentina, se evidencia en todos los modulos excepto vuelos</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the pickup location, select dates and times.</t>
+  </si>
+  <si>
+    <t>Validate that the user can enter the location to which He/She is going and the date.</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the attractions page.</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the cab reservation page.</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the type of the transfer, indicate the pick-up location, indicate the destination location and enter the dates.</t>
+  </si>
+  <si>
+    <t>Validate that the user can access the lenguage selector anywhere on the page.</t>
+  </si>
+  <si>
+    <t>Validate that the user can change the lenguage to English or French.</t>
+  </si>
+  <si>
+    <t>Validate that the user can access the currency selector anywhere on the page.</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the currency of his preference.</t>
+  </si>
+  <si>
+    <t>Validate that the user is logged in to the page.</t>
+  </si>
+  <si>
+    <t>Validate that when the user clicks on the account management dropdown, the menu is displayed.</t>
+  </si>
+  <si>
+    <t>Validate that when the user clicks on "management account" the user is redirected to account settings.</t>
+  </si>
+  <si>
+    <t>Validate that when the user clicks on "sign out" user logs out.</t>
+  </si>
+  <si>
+    <t>Assumptions</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,16 +203,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -56,17 +241,136 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -77,6 +381,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{081649D6-DF44-4160-BFE8-58378C631644}" name="Tabla1" displayName="Tabla1" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{081649D6-DF44-4160-BFE8-58378C631644}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{55007EB2-9561-4C16-8A7B-D4F9382DDF93}" name="Scope" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5E10432E-9098-4D4E-8D14-7805064EC4C3}" name="Out of reach" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,24 +657,901 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8DA754-3649-471A-A6AC-3FE28090F3F6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="12"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="9"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="12"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="6"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="12"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -369,7 +1561,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,22 +1586,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4997E7-E7E9-4DDB-AF0E-D791DECFBEB6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBDF157-B67E-47D3-9BD0-13E1010331DB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
to add scope and strategy
</commit_message>
<xml_diff>
--- a/Documentation/PTP_Jean_Ramirez_Alejandor_Marin_26092023.xlsx
+++ b/Documentation/PTP_Jean_Ramirez_Alejandor_Marin_26092023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AutomatizacionPrueba\Documents\Senasoft2023Grupo1\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Autmotizacion_Prueba\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6CE750-6E8B-4FE5-9EA5-7999D4FAF1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB04F6C-FDBE-460C-A788-93CD203642C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scope" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,166 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+  <si>
+    <t>Validate user registration module</t>
+  </si>
+  <si>
+    <t>Validate user login module</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Out of reach</t>
+  </si>
+  <si>
+    <t>Validate the following sections: booking &amp; trips, genius loyalty program, reward &amp; wallet.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: offers, trending destinations, explore Colombia, browse by property type, quick and easy trip planner, get inspiration for your next trip, saty at our top unique properties, home guests love, destinations we love, suscribe and footer.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: popular rental car companies, frequently asked questions, popular car rental destinations, suscribe and footer.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: nearby destinations, explore more destinations and footer.</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: airport taxis for any kind of trip, learn more about our airport taxi service and footer.</t>
+  </si>
+  <si>
+    <t>Not all languages will be validated in this section, only the change from Spanish to English and Spanish to French will be performed.</t>
+  </si>
+  <si>
+    <t>Not all currencies in this section will be validated, only U.S. dollar(USD) and euro(EUR) will be selected.</t>
+  </si>
+  <si>
+    <t>Validate accommodation search module</t>
+  </si>
+  <si>
+    <t>Validate flight search module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate car rental module </t>
+  </si>
+  <si>
+    <t>Validate attractions module</t>
+  </si>
+  <si>
+    <t>Validate cab reservation module</t>
+  </si>
+  <si>
+    <t>Validate language selector</t>
+  </si>
+  <si>
+    <t>Validate currency selector</t>
+  </si>
+  <si>
+    <t>Validate account management dropdown</t>
+  </si>
+  <si>
+    <t>limpiar busqueda al refrescar la pagina</t>
+  </si>
+  <si>
+    <t>si cierro sesion y doy volver, el nombre se conserva en la pantalla de bienvenida</t>
+  </si>
+  <si>
+    <t>el "a tener en cuenta" no redirecciona hacia la seccion</t>
+  </si>
+  <si>
+    <t>hotel albura no cuenta con con link de redireccion "a tener en cuenta", a pesar de tener la seccion</t>
+  </si>
+  <si>
+    <t>selector de moneda presenta error en el area de gestion de cuenta</t>
+  </si>
+  <si>
+    <t>cuando se selecciona una moneda en "gestion de cuentas" al salir del area no conserva la selección</t>
+  </si>
+  <si>
+    <t>cuando se selecciona un destino, no se borra al refrescar la pagina, ni al cerrar sesion</t>
+  </si>
+  <si>
+    <t>simbolo de moneda en monedero permanece en simbolo euro</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the accommodation search page.</t>
+  </si>
+  <si>
+    <t>selector de moneda desaparece en modulo de vuelos</t>
+  </si>
+  <si>
+    <t>The following sections will not be validated: flight type selectors, popular flights near you, trending cities, fly worldwide with booking.com and footer</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the flight page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the entered email address is not already registered </t>
+  </si>
+  <si>
+    <t>Validate that if the password entered does not have uppercase, lowercase and minimum 10 characters, do not allow to create the account.</t>
+  </si>
+  <si>
+    <t>Validate not to allow to create a user if a mandatory field is blank</t>
+  </si>
+  <si>
+    <t>Validate that the user cannot log in if he/she does not have valid credentials</t>
+  </si>
+  <si>
+    <t>Validate that the user can enter information in the search bar according to the place he/she wishes to travel to</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the departure airport, destination airport and dates.</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the car rental page.</t>
+  </si>
+  <si>
+    <t>al ingresar al selector de idiomas se observa la bandera de colombia para español de mexico y español argentina, se evidencia en todos los modulos excepto vuelos</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the pickup location, select dates and times.</t>
+  </si>
+  <si>
+    <t>Validate that the user can enter the location to which He/She is going and the date.</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the attractions page.</t>
+  </si>
+  <si>
+    <t>Validate that the user is on the cab reservation page.</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the type of the transfer, indicate the pick-up location, indicate the destination location and enter the dates.</t>
+  </si>
+  <si>
+    <t>Validate that the user can access the lenguage selector anywhere on the page.</t>
+  </si>
+  <si>
+    <t>Validate that the user can change the lenguage to English or French.</t>
+  </si>
+  <si>
+    <t>Validate that the user can access the currency selector anywhere on the page.</t>
+  </si>
+  <si>
+    <t>Validate that the user can select the currency of his preference.</t>
+  </si>
+  <si>
+    <t>Validate that the user is logged in to the page.</t>
+  </si>
+  <si>
+    <t>Validate that when the user clicks on the account management dropdown, the menu is displayed.</t>
+  </si>
+  <si>
+    <t>Validate that when the user clicks on "management account" the user is redirected to account settings.</t>
+  </si>
+  <si>
+    <t>Validate that when the user clicks on "sign out" user logs out.</t>
+  </si>
+  <si>
+    <t>Assumptions</t>
+  </si>
   <si>
     <t>Prerequisites</t>
   </si>
@@ -58,10 +217,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,12 +263,92 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -116,22 +370,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -142,6 +435,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{081649D6-DF44-4160-BFE8-58378C631644}" name="Tabla1" displayName="Tabla1" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{081649D6-DF44-4160-BFE8-58378C631644}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{55007EB2-9561-4C16-8A7B-D4F9382DDF93}" name="Scope" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5E10432E-9098-4D4E-8D14-7805064EC4C3}" name="Out of reach" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,24 +711,901 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="64" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8DA754-3649-471A-A6AC-3FE28090F3F6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="12"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="12"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="9"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="9"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="12"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="6"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="12"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -433,9 +1614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74755183-3FF7-445A-9C76-DE7DF0524AEF}">
   <dimension ref="C2:C3"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -443,18 +1622,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
+      <c r="C2" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="3:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
-        <v>1</v>
+      <c r="C3" s="18" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -462,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7B88FB-105A-4D83-ADA3-ECB983E6D61B}">
   <dimension ref="C2:C3"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,13 +1650,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="3:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
-        <v>3</v>
+      <c r="C2" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="19" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -488,24 +1666,88 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4997E7-E7E9-4DDB-AF0E-D791DECFBEB6}">
-  <dimension ref="A1"/>
+  <dimension ref="B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBDF157-B67E-47D3-9BD0-13E1010331DB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>